<commit_message>
commit all dao(NOT FINISH)
</commit_message>
<xml_diff>
--- a/StoreStock.xlsx
+++ b/StoreStock.xlsx
@@ -1,29 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
-  <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
-  <xr:revisionPtr documentId="13_ncr:1_{721E74DE-4207-48CC-B43A-12B87972D85E}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECAE35F7-70AD-4896-ADD7-927BDB3B5D11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="7" firstSheet="1" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Coffin" r:id="rId1" sheetId="1"/>
-    <sheet name="Wreath" r:id="rId2" sheetId="2"/>
-    <sheet name="Souvenirs" r:id="rId3" sheetId="4"/>
-    <sheet name="frame" r:id="rId4" sheetId="5"/>
-    <sheet name="Candles" r:id="rId5" sheetId="9"/>
-    <sheet name="Incense" r:id="rId6" sheetId="6"/>
-    <sheet name="Offering" r:id="rId7" sheetId="7"/>
-    <sheet name="SnackBox" r:id="rId8" sheetId="3"/>
-    <sheet name="Package" r:id="rId9" sheetId="8"/>
+    <sheet name="Coffin" sheetId="1" r:id="rId1"/>
+    <sheet name="Wreath" sheetId="2" r:id="rId2"/>
+    <sheet name="Souvenirs" sheetId="4" r:id="rId3"/>
+    <sheet name="frame" sheetId="5" r:id="rId4"/>
+    <sheet name="Candles" sheetId="9" r:id="rId5"/>
+    <sheet name="Incense" sheetId="6" r:id="rId6"/>
+    <sheet name="Offering" sheetId="7" r:id="rId7"/>
+    <sheet name="SnackBox" sheetId="3" r:id="rId8"/>
+    <sheet name="Package" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
   <si>
     <t>username</t>
   </si>
@@ -61,30 +61,6 @@
     <t>สี</t>
   </si>
   <si>
-    <t>แบบ F</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>1500000</t>
-  </si>
-  <si>
-    <t>ดอกไม้สด</t>
-  </si>
-  <si>
-    <t>ทดสอบ</t>
-  </si>
-  <si>
-    <t>ดอกไม้แห้ง,ดอกไม้สด</t>
-  </si>
-  <si>
-    <t>300,500</t>
-  </si>
-  <si>
-    <t>สีฟ้า,ม่วง</t>
-  </si>
-  <si>
     <t>ชุดอาหารว่าง</t>
   </si>
   <si>
@@ -143,13 +119,24 @@
   </si>
   <si>
     <t>C:\Users\User\Downloads\SnackBox5.png</t>
+  </si>
+  <si>
+    <t>ธูป&amp;เทียน</t>
+  </si>
+  <si>
+    <t>ธูปแพ็ค24ก้าน</t>
+  </si>
+  <si>
+    <t>ทดสอบบบบบบบบบบ</t>
+  </si>
+  <si>
+    <t>60</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -177,16 +164,16 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="ปกติ" xfId="0"/>
+    <cellStyle name="ปกติ" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium9" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -203,10 +190,10 @@
   <a:themeElements>
     <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -364,7 +351,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -373,13 +360,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -389,7 +376,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -398,7 +385,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -407,7 +394,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -417,12 +404,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -453,7 +440,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -472,7 +459,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -484,7 +471,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -493,43 +480,43 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="10.625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="16.875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="10.625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="12.625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="16.125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="9.25" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="12.625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="15.25" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="8.75" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="12.125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="13.5" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="7.5" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="12.125" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="12.875" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="10.75" collapsed="true"/>
+    <col min="1" max="1" width="10.625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.25" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15.25" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="8.75" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.5" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="7.5" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="12.125" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="12.875" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="10.75" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="A3:F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="27.5" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="32.75" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="13.875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="20.875" collapsed="true"/>
+    <col min="1" max="1" width="11" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.5" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="32.75" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="19" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -552,47 +539,13 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" t="s">
-        <v>19</v>
-      </c>
-    </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -601,16 +554,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="9.875" collapsed="true"/>
+    <col min="1" max="1" width="9.875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:N1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M1" sqref="M1"/>
@@ -618,7 +571,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="10.625" collapsed="true"/>
+    <col min="1" max="1" width="10.625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
@@ -663,39 +616,73 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <cols>
+    <col min="1" max="2" width="19.375" customWidth="1"/>
+    <col min="3" max="3" width="44.375" customWidth="1"/>
+    <col min="4" max="4" width="13.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="10.75" collapsed="true"/>
+    <col min="1" max="1" width="10.75" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -704,31 +691,31 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="11.25" collapsed="true"/>
+    <col min="1" max="1" width="11.25" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:E6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="10.5" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="49.125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="36.75" collapsed="true"/>
+    <col min="1" max="1" width="10.5" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="49.125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="36.75" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
         <v>8</v>
@@ -740,89 +727,89 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>21</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" t="s">
         <v>22</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C4" t="s">
         <v>23</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>25</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B5" t="s">
         <v>26</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C5" t="s">
         <v>27</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>29</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B6" t="s">
         <v>30</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C6" t="s">
         <v>31</v>
       </c>
-      <c r="D4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" t="s">
-        <v>39</v>
-      </c>
       <c r="D6" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
show img from excel
</commit_message>
<xml_diff>
--- a/StoreStock.xlsx
+++ b/StoreStock.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E1FF8C-5728-4BAB-88BD-07FBFCD47DDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Coffin" sheetId="1" r:id="rId1"/>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="73">
   <si>
     <t>ราคา</t>
   </si>
@@ -237,11 +238,17 @@
   <si>
     <t>ประกอบด้วยยยยยยยยยยยยยยยยยยยยยย</t>
   </si>
+  <si>
+    <t>รายละเอียดแบบจัดเต็ม</t>
+  </si>
+  <si>
+    <t>form_9</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -295,19 +302,25 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>198249</xdr:colOff>
+      <xdr:colOff>7749</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:rowOff>48261</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1968501</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>29515</xdr:rowOff>
+      <xdr:colOff>1592580</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="Picture"/>
+        <xdr:cNvPr id="2" name="Picture 1" descr="Picture">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -320,8 +333,52 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3747899" y="946150"/>
-          <a:ext cx="1770252" cy="1661465"/>
+          <a:off x="3490089" y="962661"/>
+          <a:ext cx="1584831" cy="149859"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2499193</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>15777</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 1" descr="Picture">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3268813" y="1173480"/>
+          <a:ext cx="2675324" cy="83820"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -334,9 +391,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -374,9 +431,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -411,7 +468,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -446,7 +503,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -619,30 +676,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:Q3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.6328125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.90625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.6328125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.6328125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.08984375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.26953125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12.6328125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.26953125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="8.7265625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12.08984375" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="13.453125" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="7.453125" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="12.08984375" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="12.90625" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="10.7265625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="10.6640625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.88671875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.6640625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.6640625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.109375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.21875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.6640625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15.21875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="8.77734375" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.109375" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.44140625" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="7.44140625" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="12.109375" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="12.88671875" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="10.77734375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -650,14 +707,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -671,7 +728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>52</v>
       </c>
@@ -685,7 +742,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>54</v>
       </c>
@@ -705,24 +762,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="A3:F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.453125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="32.7265625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.44140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="32.77734375" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="19" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.90625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.90625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.88671875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.88671875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -742,7 +799,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -768,19 +825,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K4" sqref="A1:K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.90625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="9.88671875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>56</v>
       </c>
@@ -794,7 +851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>57</v>
       </c>
@@ -808,7 +865,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>59</v>
       </c>
@@ -822,7 +879,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>61</v>
       </c>
@@ -836,7 +893,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>63</v>
       </c>
@@ -850,7 +907,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>65</v>
       </c>
@@ -864,7 +921,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>67</v>
       </c>
@@ -884,19 +941,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="N1" sqref="A1:N4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.6328125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="10.6640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>40</v>
       </c>
@@ -910,7 +967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -924,7 +981,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>43</v>
       </c>
@@ -938,7 +995,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -952,7 +1009,7 @@
         <v>1122</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -972,26 +1029,26 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="10.77734375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -999,21 +1056,21 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.26953125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="39.54296875" customWidth="1"/>
-    <col min="3" max="3" width="35.6328125" customWidth="1"/>
+    <col min="1" max="1" width="11.21875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="39.5546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="35.6640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -1027,7 +1084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -1041,7 +1098,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -1055,7 +1112,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1069,7 +1126,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1083,7 +1140,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>69</v>
       </c>
@@ -1092,6 +1149,17 @@
       </c>
       <c r="D6">
         <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7">
+        <v>256000</v>
       </c>
     </row>
   </sheetData>
@@ -1101,21 +1169,21 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="A8:D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.453125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="49.08984375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="36.7265625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="10.44140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="49.109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="36.77734375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1129,7 +1197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1143,7 +1211,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1157,7 +1225,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1171,7 +1239,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1185,7 +1253,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1199,7 +1267,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -1219,12 +1287,12 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>